<commit_message>
stdht mgn12 file relocated
</commit_message>
<xml_diff>
--- a/files/CARRIAGE/STDHT_MGN12/BOM_HextrudORT_Carriage_STDHT_MGN12.xlsx
+++ b/files/CARRIAGE/STDHT_MGN12/BOM_HextrudORT_Carriage_STDHT_MGN12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\STDHT_MGN12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDF3A57-AA51-4F80-B177-F014C419156B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3179068-52F5-4E74-AF16-3FF571E621AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2247,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2794,7 +2794,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <webPublishItems count="1">
-    <webPublishItem id="4822" divId="BOM_HextrudORT_NOVA_XCarriageMGN9_4822" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\STDHT_MGN9\BOM_HextrudORT_Carriage_STDHT_MGN12.htm" autoRepublish="1"/>
+    <webPublishItem id="4822" divId="BOM_HextrudORT_NOVA_XCarriageMGN9_4822" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\CARRIAGE\STDHT_MGN12\BOM_HextrudORT_Carriage_STDHT_MGN12.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>